<commit_message>
Update git diff protocol
</commit_message>
<xml_diff>
--- a/logDirectoryOutput.xlsx
+++ b/logDirectoryOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simeo\Documents\GitHub\bitcoin-version-compare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Simeon\Documents\GitHub\bitcoin-version-compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6A19E8-E50B-41AC-89AF-9FFE97990EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D13B3DC-CE64-4012-A160-7EC4EA57FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="1020" windowWidth="21870" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logDirectoryOutput" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,6 @@
     <t>Size all files (B)</t>
   </si>
   <si>
-    <t>Num code files (cpp, py, c, h, sh)</t>
-  </si>
-  <si>
     <t>Size code files (B)</t>
   </si>
   <si>
@@ -262,12 +259,6 @@
     <t>.cpp (516), .h (450), .py (233), .md (180), .png (93), .json (92), .cc (89), .ts (89), .sh (73),  (65), .mk (38), .hex (28), .patch (26), .in (23), .svg (21), .c (19), .ui (19), .vcxproj (17), .m4 (16), .yml (13), .include (13), .txt (8), .1 (6), .rc (6), .sage (6), .am (5), .xpm (5), .ac (3), .bash-completion (3), .bash (3), .conf (3), .ico (3), .mm (3), .targets (2), .pro (2), .bmp (2), .raw (2), .capnp (2), .html (2), .qrc (2), .yapf (1), .sln (1), .supp (1), .scm (1), .init (1), .openrc (1), .openrcconf (1), .service (1), .plist (1), .cfg (1), .cert (1), .guess (1), .sub (1), .cmake (1), .xml (1), .gradle (1), .properties (1), .java (1), .xlf (1), .ttf (1), .icns (1), .Dockerfile (1), .s (1), .csv (1)</t>
   </si>
   <si>
-    <t>Ratio all bytes changed (B)</t>
-  </si>
-  <si>
-    <t>Code changed bytes (B)</t>
-  </si>
-  <si>
     <t>Unit = Bytes</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
   </si>
   <si>
     <t>Metadata / high level overview</t>
-  </si>
-  <si>
-    <t>Bitcoin Version</t>
   </si>
   <si>
     <t>Comparison across all files</t>
@@ -297,6 +285,18 @@
   <si>
     <t>Comparison across code files
 (.cpp, .py, .c, .h, .sh)</t>
+  </si>
+  <si>
+    <t>Bitcoin Core Version</t>
+  </si>
+  <si>
+    <t>Num code files (cpp, py, c, h, sh, sol, go, c, js, java)</t>
+  </si>
+  <si>
+    <t>Ratio all bytes changed</t>
+  </si>
+  <si>
+    <t>Code changed bytes</t>
   </si>
 </sst>
 </file>
@@ -1206,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1230,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1239,164 +1239,164 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1083</v>
+      </c>
+      <c r="C2" s="5">
+        <v>14903579</v>
+      </c>
+      <c r="D2" s="8">
+        <v>580</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4721951</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1095</v>
-      </c>
-      <c r="C2" s="5">
-        <v>14620679</v>
-      </c>
-      <c r="D2" s="8">
-        <v>568</v>
-      </c>
-      <c r="E2" s="5">
-        <v>4165742</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="8">
-        <v>1099</v>
+        <v>1087</v>
       </c>
       <c r="C3" s="5">
-        <v>14808599</v>
+        <v>15095814</v>
       </c>
       <c r="D3" s="8">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="E3" s="5">
-        <v>4187910</v>
+        <v>4744552</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="7">
-        <v>7876</v>
+        <v>7899</v>
       </c>
       <c r="H3" s="7">
-        <v>3561</v>
+        <v>3584</v>
       </c>
       <c r="I3" s="8">
         <v>102</v>
       </c>
       <c r="J3" s="4">
-        <v>9.2811646951774296E-2</v>
+        <v>9.3836246550137906E-2</v>
       </c>
       <c r="K3" s="5">
-        <v>6471407</v>
+        <v>6635724</v>
       </c>
       <c r="L3" s="4">
-        <v>0.43700332489251598</v>
+        <v>0.43957377853224699</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="7">
         <v>777</v>
@@ -1408,39 +1408,39 @@
         <v>28</v>
       </c>
       <c r="Q3" s="4">
-        <v>4.9036777583187301E-2</v>
+        <v>4.8027444253859297E-2</v>
       </c>
       <c r="R3" s="5">
-        <v>638374</v>
+        <v>655429</v>
       </c>
       <c r="S3" s="4">
-        <v>0.15243259764417</v>
+        <v>0.138143495950724</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8">
-        <v>1099</v>
+        <v>1087</v>
       </c>
       <c r="C4" s="5">
-        <v>14946005</v>
+        <v>15236204</v>
       </c>
       <c r="D4" s="8">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="E4" s="5">
-        <v>4188532</v>
+        <v>4745189</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" s="7">
         <v>3687</v>
@@ -1452,16 +1452,16 @@
         <v>80</v>
       </c>
       <c r="J4" s="4">
-        <v>7.27934485896269E-2</v>
+        <v>7.3597056117755202E-2</v>
       </c>
       <c r="K4" s="5">
-        <v>5857121</v>
+        <v>6004849</v>
       </c>
       <c r="L4" s="4">
-        <v>0.39188539010926299</v>
+        <v>0.39411713048735703</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" s="7">
         <v>23</v>
@@ -1473,60 +1473,60 @@
         <v>5</v>
       </c>
       <c r="Q4" s="4">
-        <v>8.75656742556917E-3</v>
+        <v>8.5763293310463107E-3</v>
       </c>
       <c r="R4" s="5">
-        <v>82531</v>
+        <v>84831</v>
       </c>
       <c r="S4" s="4">
-        <v>1.97040395059653E-2</v>
+        <v>1.78772647411936E-2</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8">
-        <v>1099</v>
+        <v>1087</v>
       </c>
       <c r="C5" s="5">
-        <v>14984493</v>
+        <v>15275510</v>
       </c>
       <c r="D5" s="8">
-        <v>571</v>
+        <v>583</v>
       </c>
       <c r="E5" s="5">
-        <v>4194019</v>
+        <v>4750771</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="7">
-        <v>4451</v>
+        <v>4534</v>
       </c>
       <c r="H5" s="7">
-        <v>3633</v>
+        <v>3716</v>
       </c>
       <c r="I5" s="8">
         <v>99</v>
       </c>
       <c r="J5" s="4">
-        <v>9.0081892629663304E-2</v>
+        <v>9.1076356945722095E-2</v>
       </c>
       <c r="K5" s="5">
-        <v>6424300</v>
+        <v>6585714</v>
       </c>
       <c r="L5" s="4">
-        <v>0.42872988762449199</v>
+        <v>0.431128911571528</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" s="7">
         <v>151</v>
@@ -1538,39 +1538,39 @@
         <v>29</v>
       </c>
       <c r="Q5" s="4">
-        <v>5.0788091068301199E-2</v>
+        <v>4.9742710120068603E-2</v>
       </c>
       <c r="R5" s="5">
-        <v>769042</v>
+        <v>789491</v>
       </c>
       <c r="S5" s="4">
-        <v>0.18336636052435601</v>
+        <v>0.16618165767198601</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8">
-        <v>1106</v>
+        <v>1094</v>
       </c>
       <c r="C6" s="5">
-        <v>15052095</v>
+        <v>15344555</v>
       </c>
       <c r="D6" s="8">
-        <v>573</v>
+        <v>585</v>
       </c>
       <c r="E6" s="5">
-        <v>4205693</v>
+        <v>4772802</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="7">
         <v>1897</v>
@@ -1582,125 +1582,125 @@
         <v>62</v>
       </c>
       <c r="J6" s="4">
-        <v>5.6057866184448399E-2</v>
+        <v>5.6672760511882997E-2</v>
       </c>
       <c r="K6" s="5">
-        <v>1746251</v>
+        <v>1791224</v>
       </c>
       <c r="L6" s="4">
-        <v>0.11601381734569099</v>
+        <v>0.11673352534498301</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" s="7">
-        <v>519</v>
+        <v>635</v>
       </c>
       <c r="O6" s="7">
         <v>264</v>
       </c>
       <c r="P6" s="8">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q6" s="4">
-        <v>5.23560209424083E-2</v>
+        <v>5.4700854700854701E-2</v>
       </c>
       <c r="R6" s="5">
-        <v>624440</v>
+        <v>698365</v>
       </c>
       <c r="S6" s="4">
-        <v>0.148474936235241</v>
+        <v>0.14632180425670199</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1141</v>
+      </c>
+      <c r="C7" s="5">
+        <v>17029718</v>
+      </c>
+      <c r="D7" s="8">
+        <v>625</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5293803</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>37242</v>
+      </c>
+      <c r="H7" s="7">
+        <v>24939</v>
+      </c>
+      <c r="I7" s="8">
+        <v>767</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.67221735319894804</v>
+      </c>
+      <c r="K7" s="5">
+        <v>12749790</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.74867886831713804</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="7">
+        <v>23971</v>
+      </c>
+      <c r="O7" s="7">
+        <v>9801</v>
+      </c>
+      <c r="P7" s="8">
+        <v>443</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0.70879999999999999</v>
+      </c>
+      <c r="R7" s="5">
+        <v>4055688</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0.76611993306135495</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1154</v>
-      </c>
-      <c r="C7" s="5">
-        <v>16729098</v>
-      </c>
-      <c r="D7" s="8">
-        <v>615</v>
-      </c>
-      <c r="E7" s="5">
-        <v>4718261</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="7">
-        <v>37157</v>
-      </c>
-      <c r="H7" s="7">
-        <v>24777</v>
-      </c>
-      <c r="I7" s="8">
-        <v>773</v>
-      </c>
-      <c r="J7" s="4">
-        <v>0.66984402079722705</v>
-      </c>
-      <c r="K7" s="5">
-        <v>12486528</v>
-      </c>
-      <c r="L7" s="4">
-        <v>0.746395771009291</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="7">
-        <v>23678</v>
-      </c>
-      <c r="O7" s="7">
-        <v>9482</v>
-      </c>
-      <c r="P7" s="8">
-        <v>439</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>0.71382113821138204</v>
-      </c>
-      <c r="R7" s="5">
-        <v>3744208</v>
-      </c>
-      <c r="S7" s="4">
-        <v>0.79355677865213403</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="8">
-        <v>1159</v>
+        <v>1146</v>
       </c>
       <c r="C8" s="5">
-        <v>16779491</v>
+        <v>17081012</v>
       </c>
       <c r="D8" s="8">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="E8" s="5">
-        <v>4734939</v>
+        <v>5320941</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="7">
         <v>1366</v>
@@ -1712,450 +1712,450 @@
         <v>65</v>
       </c>
       <c r="J8" s="4">
-        <v>5.6082830025884302E-2</v>
+        <v>5.6719022687608998E-2</v>
       </c>
       <c r="K8" s="5">
-        <v>1127026</v>
+        <v>1155791</v>
       </c>
       <c r="L8" s="4">
-        <v>6.7166876516099303E-2</v>
+        <v>6.7665253089219696E-2</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N8" s="7">
-        <v>643</v>
+        <v>757</v>
       </c>
       <c r="O8" s="7">
         <v>281</v>
       </c>
       <c r="P8" s="8">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q8" s="4">
-        <v>5.9967585089140997E-2</v>
+        <v>6.2200956937799E-2</v>
       </c>
       <c r="R8" s="5">
-        <v>827752</v>
+        <v>909461</v>
       </c>
       <c r="S8" s="4">
-        <v>0.17481788044154301</v>
+        <v>0.17092108331965999</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1270</v>
+      </c>
+      <c r="C9" s="5">
+        <v>19038621</v>
+      </c>
+      <c r="D9" s="8">
+        <v>728</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6159950</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="7">
+        <v>59370</v>
+      </c>
+      <c r="H9" s="7">
+        <v>22002</v>
+      </c>
+      <c r="I9" s="8">
+        <v>803</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.63228346456692897</v>
+      </c>
+      <c r="K9" s="5">
+        <v>13555940</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0.71202320798339302</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="7">
+        <v>32242</v>
+      </c>
+      <c r="O9" s="7">
+        <v>8848</v>
+      </c>
+      <c r="P9" s="8">
+        <v>493</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.67719780219780201</v>
+      </c>
+      <c r="R9" s="5">
+        <v>4773321</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0.77489606246803899</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="8">
-        <v>1286</v>
-      </c>
-      <c r="C9" s="5">
-        <v>18707622</v>
-      </c>
-      <c r="D9" s="8">
-        <v>678</v>
-      </c>
-      <c r="E9" s="5">
-        <v>5550438</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="7">
-        <v>59570</v>
-      </c>
-      <c r="H9" s="7">
-        <v>21951</v>
-      </c>
-      <c r="I9" s="8">
-        <v>808</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0.62830482115085495</v>
-      </c>
-      <c r="K9" s="5">
-        <v>13262892</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0.70895659533851996</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N9" s="7">
-        <v>32067</v>
-      </c>
-      <c r="O9" s="7">
-        <v>8814</v>
-      </c>
-      <c r="P9" s="8">
-        <v>448</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>0.66076696165191695</v>
-      </c>
-      <c r="R9" s="5">
-        <v>4430289</v>
-      </c>
-      <c r="S9" s="4">
-        <v>0.79818727819318003</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="8">
-        <v>1299</v>
+        <v>1283</v>
       </c>
       <c r="C10" s="5">
-        <v>19029384</v>
+        <v>19368444</v>
       </c>
       <c r="D10" s="8">
-        <v>685</v>
+        <v>735</v>
       </c>
       <c r="E10" s="5">
-        <v>5667895</v>
+        <v>6292977</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="7">
-        <v>9390</v>
+        <v>9391</v>
       </c>
       <c r="H10" s="7">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="I10" s="8">
         <v>93</v>
       </c>
       <c r="J10" s="4">
-        <v>7.1593533487297897E-2</v>
+        <v>7.2486360093530794E-2</v>
       </c>
       <c r="K10" s="5">
-        <v>3893945</v>
+        <v>3991734</v>
       </c>
       <c r="L10" s="4">
-        <v>0.20462801108012699</v>
+        <v>0.206094717779084</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" s="7">
-        <v>2741</v>
+        <v>2879</v>
       </c>
       <c r="O10" s="7">
         <v>148</v>
       </c>
       <c r="P10" s="8">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="4">
-        <v>6.5693430656934296E-2</v>
+        <v>6.3945578231292502E-2</v>
       </c>
       <c r="R10" s="5">
-        <v>1182273</v>
+        <v>1285479</v>
       </c>
       <c r="S10" s="4">
-        <v>0.20859119655533401</v>
+        <v>0.20427200035849399</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1346</v>
+      </c>
+      <c r="C11" s="5">
+        <v>16521038</v>
+      </c>
+      <c r="D11" s="8">
+        <v>773</v>
+      </c>
+      <c r="E11" s="5">
+        <v>6952935</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="7">
+        <v>41432</v>
+      </c>
+      <c r="H11" s="7">
+        <v>82986</v>
+      </c>
+      <c r="I11" s="8">
+        <v>610</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.45319465081723598</v>
+      </c>
+      <c r="K11" s="5">
+        <v>10459833</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.63312202296247899</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="7">
+        <v>23715</v>
+      </c>
+      <c r="O11" s="7">
+        <v>6716</v>
+      </c>
+      <c r="P11" s="8">
+        <v>364</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0.47089262613195298</v>
+      </c>
+      <c r="R11" s="5">
+        <v>4492391</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0.64611433876485203</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U11" t="s">
         <v>32</v>
-      </c>
-      <c r="B11" s="8">
-        <v>1363</v>
-      </c>
-      <c r="C11" s="5">
-        <v>16225523</v>
-      </c>
-      <c r="D11" s="8">
-        <v>719</v>
-      </c>
-      <c r="E11" s="5">
-        <v>6244200</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="7">
-        <v>38487</v>
-      </c>
-      <c r="H11" s="7">
-        <v>80008</v>
-      </c>
-      <c r="I11" s="8">
-        <v>619</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0.454145267791636</v>
-      </c>
-      <c r="K11" s="5">
-        <v>10230288</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0.630505901104081</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N11" s="7">
-        <v>21292</v>
-      </c>
-      <c r="O11" s="7">
-        <v>6669</v>
-      </c>
-      <c r="P11" s="8">
-        <v>355</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>0.49374130737134903</v>
-      </c>
-      <c r="R11" s="5">
-        <v>4078487</v>
-      </c>
-      <c r="S11" s="4">
-        <v>0.65316405624419405</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1365</v>
+      </c>
+      <c r="C12" s="5">
+        <v>17311593</v>
+      </c>
+      <c r="D12" s="8">
+        <v>789</v>
+      </c>
+      <c r="E12" s="5">
+        <v>7209482</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="7">
+        <v>21294</v>
+      </c>
+      <c r="H12" s="7">
+        <v>2742</v>
+      </c>
+      <c r="I12" s="8">
+        <v>246</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0.18021978021978</v>
+      </c>
+      <c r="K12" s="5">
+        <v>7827415</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.45214874217525702</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="7">
+        <v>5039</v>
+      </c>
+      <c r="O12" s="7">
+        <v>784</v>
+      </c>
+      <c r="P12" s="8">
+        <v>134</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>0.16983523447401699</v>
+      </c>
+      <c r="R12" s="5">
+        <v>2593338</v>
+      </c>
+      <c r="S12" s="4">
+        <v>0.359712112465222</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="8">
-        <v>1383</v>
-      </c>
-      <c r="C12" s="5">
-        <v>17000206</v>
-      </c>
-      <c r="D12" s="8">
-        <v>724</v>
-      </c>
-      <c r="E12" s="5">
-        <v>6385859</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="7">
-        <v>21016</v>
-      </c>
-      <c r="H12" s="7">
-        <v>2433</v>
-      </c>
-      <c r="I12" s="8">
-        <v>247</v>
-      </c>
-      <c r="J12" s="4">
-        <v>0.17859725234996299</v>
-      </c>
-      <c r="K12" s="5">
-        <v>7642750</v>
-      </c>
-      <c r="L12" s="4">
-        <v>0.44956808170442097</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N12" s="7">
-        <v>3531</v>
-      </c>
-      <c r="O12" s="7">
-        <v>782</v>
-      </c>
-      <c r="P12" s="8">
-        <v>121</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>0.16712707182320399</v>
-      </c>
-      <c r="R12" s="5">
-        <v>2235961</v>
-      </c>
-      <c r="S12" s="4">
-        <v>0.35014255717202603</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1375</v>
+      </c>
+      <c r="C13" s="5">
+        <v>18039442</v>
+      </c>
+      <c r="D13" s="8">
+        <v>791</v>
+      </c>
+      <c r="E13" s="5">
+        <v>7291309</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="7">
+        <v>20894</v>
+      </c>
+      <c r="H13" s="7">
+        <v>2442</v>
+      </c>
+      <c r="I13" s="8">
+        <v>197</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0.143272727272727</v>
+      </c>
+      <c r="K13" s="5">
+        <v>5714943</v>
+      </c>
+      <c r="L13" s="4">
+        <v>0.31680264833025301</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="7">
+        <v>3165</v>
+      </c>
+      <c r="O13" s="7">
+        <v>645</v>
+      </c>
+      <c r="P13" s="8">
+        <v>124</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>0.15676359039190799</v>
+      </c>
+      <c r="R13" s="5">
+        <v>2846341</v>
+      </c>
+      <c r="S13" s="4">
+        <v>0.39037448556905202</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U13" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1391</v>
-      </c>
-      <c r="C13" s="5">
-        <v>17703466</v>
-      </c>
-      <c r="D13" s="8">
-        <v>723</v>
-      </c>
-      <c r="E13" s="5">
-        <v>6427300</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G13" s="7">
-        <v>20573</v>
-      </c>
-      <c r="H13" s="7">
-        <v>2311</v>
-      </c>
-      <c r="I13" s="8">
-        <v>196</v>
-      </c>
-      <c r="J13" s="4">
-        <v>0.140905823148813</v>
-      </c>
-      <c r="K13" s="5">
-        <v>5572840</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0.31478807596207398</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N13" s="7">
-        <v>2381</v>
-      </c>
-      <c r="O13" s="7">
-        <v>618</v>
-      </c>
-      <c r="P13" s="8">
-        <v>118</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>0.16320885200553201</v>
-      </c>
-      <c r="R13" s="5">
-        <v>2621440</v>
-      </c>
-      <c r="S13" s="4">
-        <v>0.40786022124375698</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1453</v>
+      </c>
+      <c r="C14" s="5">
+        <v>20121295</v>
+      </c>
+      <c r="D14" s="8">
+        <v>857</v>
+      </c>
+      <c r="E14" s="5">
+        <v>7817838</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="7">
+        <v>52061</v>
+      </c>
+      <c r="H14" s="7">
+        <v>24638</v>
+      </c>
+      <c r="I14" s="8">
+        <v>713</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0.49070887818306902</v>
+      </c>
+      <c r="K14" s="5">
+        <v>13555156</v>
+      </c>
+      <c r="L14" s="4">
+        <v>0.67367214684740695</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="7">
+        <v>27125</v>
+      </c>
+      <c r="O14" s="7">
+        <v>13455</v>
+      </c>
+      <c r="P14" s="8">
+        <v>495</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>0.57759626604434</v>
+      </c>
+      <c r="R14" s="5">
+        <v>5656574</v>
+      </c>
+      <c r="S14" s="4">
+        <v>0.72354709831541597</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U14" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="8">
-        <v>1468</v>
-      </c>
-      <c r="C14" s="5">
-        <v>19755185</v>
-      </c>
-      <c r="D14" s="8">
-        <v>777</v>
-      </c>
-      <c r="E14" s="5">
-        <v>6920616</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="7">
-        <v>51875</v>
-      </c>
-      <c r="H14" s="7">
-        <v>24470</v>
-      </c>
-      <c r="I14" s="8">
-        <v>722</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0.49182561307901901</v>
-      </c>
-      <c r="K14" s="5">
-        <v>13245553</v>
-      </c>
-      <c r="L14" s="4">
-        <v>0.67048488789145699</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N14" s="7">
-        <v>26620</v>
-      </c>
-      <c r="O14" s="7">
-        <v>13381</v>
-      </c>
-      <c r="P14" s="8">
-        <v>475</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>0.61132561132561103</v>
-      </c>
-      <c r="R14" s="5">
-        <v>5392595</v>
-      </c>
-      <c r="S14" s="4">
-        <v>0.77920737113574801</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="8">
-        <v>1468</v>
+        <v>1453</v>
       </c>
       <c r="C15" s="5">
-        <v>19779824</v>
+        <v>20146738</v>
       </c>
       <c r="D15" s="8">
-        <v>777</v>
+        <v>857</v>
       </c>
       <c r="E15" s="5">
-        <v>6928159</v>
+        <v>7826952</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G15" s="7">
         <v>1710</v>
@@ -2167,60 +2167,60 @@
         <v>48</v>
       </c>
       <c r="J15" s="4">
-        <v>3.2697547683923703E-2</v>
+        <v>3.3035099793530601E-2</v>
       </c>
       <c r="K15" s="5">
-        <v>2807832</v>
+        <v>2877042</v>
       </c>
       <c r="L15" s="4">
-        <v>0.141954347015423</v>
+        <v>0.142804358700649</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N15" s="7">
-        <v>223</v>
+        <v>259</v>
       </c>
       <c r="O15" s="7">
         <v>64</v>
       </c>
       <c r="P15" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q15" s="4">
-        <v>3.2175032175032099E-2</v>
+        <v>3.0338389731621899E-2</v>
       </c>
       <c r="R15" s="5">
-        <v>849533</v>
+        <v>890985</v>
       </c>
       <c r="S15" s="4">
-        <v>0.122620309378003</v>
+        <v>0.113835500715987</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="8">
-        <v>1469</v>
+        <v>1454</v>
       </c>
       <c r="C16" s="5">
-        <v>19899500</v>
+        <v>20269075</v>
       </c>
       <c r="D16" s="8">
-        <v>777</v>
+        <v>857</v>
       </c>
       <c r="E16" s="5">
-        <v>6932908</v>
+        <v>7831813</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="7">
         <v>2944</v>
@@ -2232,16 +2232,16 @@
         <v>41</v>
       </c>
       <c r="J16" s="4">
-        <v>2.7910142954390701E-2</v>
+        <v>2.8198074277854101E-2</v>
       </c>
       <c r="K16" s="5">
-        <v>2405978</v>
+        <v>2466483</v>
       </c>
       <c r="L16" s="4">
-        <v>0.120906454936053</v>
+        <v>0.12168700347697101</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N16" s="7">
         <v>135</v>
@@ -2253,39 +2253,39 @@
         <v>10</v>
       </c>
       <c r="Q16" s="4">
-        <v>1.28700128700128E-2</v>
+        <v>1.1668611435239199E-2</v>
       </c>
       <c r="R16" s="5">
-        <v>400907</v>
+        <v>411977</v>
       </c>
       <c r="S16" s="4">
-        <v>5.7826672443944099E-2</v>
+        <v>5.2603017972977603E-2</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="8">
-        <v>1470</v>
+        <v>1455</v>
       </c>
       <c r="C17" s="5">
-        <v>19919589</v>
+        <v>20289747</v>
       </c>
       <c r="D17" s="8">
-        <v>778</v>
+        <v>858</v>
       </c>
       <c r="E17" s="5">
-        <v>6948174</v>
+        <v>7847503</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="7">
         <v>902</v>
@@ -2297,16 +2297,16 @@
         <v>42</v>
       </c>
       <c r="J17" s="4">
-        <v>2.8571428571428501E-2</v>
+        <v>2.88659793814433E-2</v>
       </c>
       <c r="K17" s="5">
-        <v>1166387</v>
+        <v>1196318</v>
       </c>
       <c r="L17" s="4">
-        <v>5.8554772390133097E-2</v>
+        <v>5.8961701198146997E-2</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N17" s="7">
         <v>656</v>
@@ -2318,125 +2318,125 @@
         <v>27</v>
       </c>
       <c r="Q17" s="4">
-        <v>3.4704370179948499E-2</v>
+        <v>3.1468531468531402E-2</v>
       </c>
       <c r="R17" s="5">
-        <v>1001480</v>
+        <v>1026360</v>
       </c>
       <c r="S17" s="4">
-        <v>0.144135711051565</v>
+        <v>0.130788099093431</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1506</v>
+      </c>
+      <c r="C18" s="5">
+        <v>21479913</v>
+      </c>
+      <c r="D18" s="8">
+        <v>886</v>
+      </c>
+      <c r="E18" s="5">
+        <v>8231328</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="7">
+        <v>45568</v>
+      </c>
+      <c r="H18" s="7">
+        <v>19414</v>
+      </c>
+      <c r="I18" s="8">
+        <v>670</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0.44488711819389098</v>
+      </c>
+      <c r="K18" s="5">
+        <v>11591023</v>
+      </c>
+      <c r="L18" s="4">
+        <v>0.53962150591578195</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" s="7">
+        <v>25711</v>
+      </c>
+      <c r="O18" s="7">
+        <v>14301</v>
+      </c>
+      <c r="P18" s="8">
+        <v>512</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>0.57787810383747096</v>
+      </c>
+      <c r="R18" s="5">
+        <v>6559860</v>
+      </c>
+      <c r="S18" s="4">
+        <v>0.79693823402493502</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U18" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" s="8">
-        <v>1521</v>
-      </c>
-      <c r="C18" s="5">
-        <v>21083710</v>
-      </c>
-      <c r="D18" s="8">
-        <v>806</v>
-      </c>
-      <c r="E18" s="5">
-        <v>7322542</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="7">
-        <v>45552</v>
-      </c>
-      <c r="H18" s="7">
-        <v>19397</v>
-      </c>
-      <c r="I18" s="8">
-        <v>671</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0.44115713346482499</v>
-      </c>
-      <c r="K18" s="5">
-        <v>11319794</v>
-      </c>
-      <c r="L18" s="4">
-        <v>0.53689763329129403</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N18" s="7">
-        <v>25626</v>
-      </c>
-      <c r="O18" s="7">
-        <v>14262</v>
-      </c>
-      <c r="P18" s="8">
-        <v>485</v>
-      </c>
-      <c r="Q18" s="4">
-        <v>0.60173697270471405</v>
-      </c>
-      <c r="R18" s="5">
-        <v>5955511</v>
-      </c>
-      <c r="S18" s="4">
-        <v>0.81331196188427402</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U18" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="8">
-        <v>1521</v>
+        <v>1506</v>
       </c>
       <c r="C19" s="5">
-        <v>21101934</v>
+        <v>21499179</v>
       </c>
       <c r="D19" s="8">
-        <v>806</v>
+        <v>886</v>
       </c>
       <c r="E19" s="5">
-        <v>7322471</v>
+        <v>8231257</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" s="7">
-        <v>1996</v>
+        <v>2062</v>
       </c>
       <c r="H19" s="7">
-        <v>954</v>
+        <v>1020</v>
       </c>
       <c r="I19" s="8">
         <v>19</v>
       </c>
       <c r="J19" s="4">
-        <v>1.24917817225509E-2</v>
+        <v>1.26162018592297E-2</v>
       </c>
       <c r="K19" s="5">
-        <v>1389889</v>
+        <v>1424866</v>
       </c>
       <c r="L19" s="4">
-        <v>6.5865479438993596E-2</v>
+        <v>6.6275368003587395E-2</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N19" s="7">
         <v>3</v>
@@ -2448,39 +2448,39 @@
         <v>2</v>
       </c>
       <c r="Q19" s="4">
-        <v>2.48138957816377E-3</v>
+        <v>2.2573363431151201E-3</v>
       </c>
       <c r="R19" s="5">
-        <v>38348</v>
+        <v>39362</v>
       </c>
       <c r="S19" s="4">
-        <v>5.2370299588759004E-3</v>
+        <v>4.7820156751271397E-3</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="8">
-        <v>1526</v>
+        <v>1511</v>
       </c>
       <c r="C20" s="5">
-        <v>21257097</v>
+        <v>21657365</v>
       </c>
       <c r="D20" s="8">
-        <v>808</v>
+        <v>889</v>
       </c>
       <c r="E20" s="5">
-        <v>7402504</v>
+        <v>8315517</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" s="7">
         <v>4841</v>
@@ -2492,81 +2492,81 @@
         <v>162</v>
       </c>
       <c r="J20" s="4">
-        <v>0.10615989515072</v>
+        <v>0.107213765718067</v>
       </c>
       <c r="K20" s="5">
-        <v>2968877</v>
+        <v>3040622</v>
       </c>
       <c r="L20" s="4">
-        <v>0.13966521392831699</v>
+        <v>0.14039667337185199</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N20" s="7">
-        <v>3567</v>
+        <v>3611</v>
       </c>
       <c r="O20" s="7">
         <v>1664</v>
       </c>
       <c r="P20" s="8">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="Q20" s="4">
-        <v>0.17821782178217799</v>
+        <v>0.16422947131608501</v>
       </c>
       <c r="R20" s="5">
-        <v>2733955</v>
+        <v>2822954</v>
       </c>
       <c r="S20" s="4">
-        <v>0.36932840563139102</v>
+        <v>0.33948027524927099</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="8">
-        <v>1528</v>
+        <v>1511</v>
       </c>
       <c r="C21" s="5">
-        <v>21255041</v>
+        <v>21650572</v>
       </c>
       <c r="D21" s="8">
-        <v>808</v>
+        <v>889</v>
       </c>
       <c r="E21" s="5">
-        <v>7404369</v>
+        <v>8317408</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21" s="7">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="H21" s="7">
         <v>266</v>
       </c>
       <c r="I21" s="8">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J21" s="4">
-        <v>1.50523560209424E-2</v>
+        <v>1.38980807412309E-2</v>
       </c>
       <c r="K21" s="5">
-        <v>629636</v>
+        <v>640308</v>
       </c>
       <c r="L21" s="4">
-        <v>2.96229021623623E-2</v>
+        <v>2.9574645880025702E-2</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N21" s="7">
         <v>70</v>
@@ -2578,169 +2578,169 @@
         <v>13</v>
       </c>
       <c r="Q21" s="4">
-        <v>1.6089108910890999E-2</v>
+        <v>1.4623172103487E-2</v>
       </c>
       <c r="R21" s="5">
-        <v>526970</v>
+        <v>539218</v>
       </c>
       <c r="S21" s="4">
-        <v>7.1170142925075702E-2</v>
+        <v>6.4830052824148998E-2</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1535</v>
+      </c>
+      <c r="C22" s="5">
+        <v>22077610</v>
+      </c>
+      <c r="D22" s="8">
+        <v>929</v>
+      </c>
+      <c r="E22" s="5">
+        <v>8554175</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7">
+        <v>63215</v>
+      </c>
+      <c r="H22" s="7">
+        <v>23511</v>
+      </c>
+      <c r="I22" s="8">
+        <v>873</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0.56872964169381102</v>
+      </c>
+      <c r="K22" s="5">
+        <v>15673687</v>
+      </c>
+      <c r="L22" s="4">
+        <v>0.70993585809333504</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N22" s="7">
+        <v>18565</v>
+      </c>
+      <c r="O22" s="7">
+        <v>12632</v>
+      </c>
+      <c r="P22" s="8">
+        <v>626</v>
+      </c>
+      <c r="Q22" s="4">
+        <v>0.67384284176533904</v>
+      </c>
+      <c r="R22" s="5">
+        <v>6896550</v>
+      </c>
+      <c r="S22" s="4">
+        <v>0.80622035438835404</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U22" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" s="8">
-        <v>1549</v>
-      </c>
-      <c r="C22" s="5">
-        <v>21636398</v>
-      </c>
-      <c r="D22" s="8">
-        <v>841</v>
-      </c>
-      <c r="E22" s="5">
-        <v>7631342</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G22" s="7">
-        <v>62761</v>
-      </c>
-      <c r="H22" s="7">
-        <v>23191</v>
-      </c>
-      <c r="I22" s="8">
-        <v>879</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0.56746287927695205</v>
-      </c>
-      <c r="K22" s="5">
-        <v>15292771</v>
-      </c>
-      <c r="L22" s="4">
-        <v>0.70680762112066897</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N22" s="7">
-        <v>18056</v>
-      </c>
-      <c r="O22" s="7">
-        <v>12256</v>
-      </c>
-      <c r="P22" s="8">
-        <v>602</v>
-      </c>
-      <c r="Q22" s="4">
-        <v>0.71581450653983303</v>
-      </c>
-      <c r="R22" s="5">
-        <v>6290997</v>
-      </c>
-      <c r="S22" s="4">
-        <v>0.82436313298499797</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U22" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1536</v>
+      </c>
+      <c r="C23" s="5">
+        <v>22265347</v>
+      </c>
+      <c r="D23" s="8">
+        <v>931</v>
+      </c>
+      <c r="E23" s="5">
+        <v>8582456</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="7">
+        <v>10433</v>
+      </c>
+      <c r="H23" s="7">
+        <v>6053</v>
+      </c>
+      <c r="I23" s="8">
+        <v>121</v>
+      </c>
+      <c r="J23" s="4">
+        <v>7.8776041666666602E-2</v>
+      </c>
+      <c r="K23" s="5">
+        <v>7654871</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0.34380200766689101</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" s="7">
+        <v>674</v>
+      </c>
+      <c r="O23" s="7">
+        <v>207</v>
+      </c>
+      <c r="P23" s="8">
+        <v>59</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>6.3372717508055801E-2</v>
+      </c>
+      <c r="R23" s="5">
+        <v>1843785</v>
+      </c>
+      <c r="S23" s="4">
+        <v>0.21483186164892601</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U23" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" s="8">
-        <v>1552</v>
-      </c>
-      <c r="C23" s="5">
-        <v>21824336</v>
-      </c>
-      <c r="D23" s="8">
-        <v>843</v>
-      </c>
-      <c r="E23" s="5">
-        <v>7649031</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G23" s="7">
-        <v>10153</v>
-      </c>
-      <c r="H23" s="7">
-        <v>5670</v>
-      </c>
-      <c r="I23" s="8">
-        <v>124</v>
-      </c>
-      <c r="J23" s="4">
-        <v>7.9896907216494797E-2</v>
-      </c>
-      <c r="K23" s="5">
-        <v>7487886</v>
-      </c>
-      <c r="L23" s="4">
-        <v>0.34309799849122502</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N23" s="7">
-        <v>621</v>
-      </c>
-      <c r="O23" s="7">
-        <v>202</v>
-      </c>
-      <c r="P23" s="8">
-        <v>57</v>
-      </c>
-      <c r="Q23" s="4">
-        <v>6.76156583629893E-2</v>
-      </c>
-      <c r="R23" s="5">
-        <v>1663849</v>
-      </c>
-      <c r="S23" s="4">
-        <v>0.217524154366742</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="8">
-        <v>1552</v>
+        <v>1536</v>
       </c>
       <c r="C24" s="5">
-        <v>21824497</v>
+        <v>22265548</v>
       </c>
       <c r="D24" s="8">
-        <v>843</v>
+        <v>931</v>
       </c>
       <c r="E24" s="5">
-        <v>7650831</v>
+        <v>8584335</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G24" s="7">
         <v>351</v>
@@ -2752,16 +2752,16 @@
         <v>70</v>
       </c>
       <c r="J24" s="4">
-        <v>4.5103092783505098E-2</v>
+        <v>4.5572916666666602E-2</v>
       </c>
       <c r="K24" s="5">
-        <v>1905224</v>
+        <v>1953342</v>
       </c>
       <c r="L24" s="4">
-        <v>8.7297498769387402E-2</v>
+        <v>8.7729347600157798E-2</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N24" s="7">
         <v>294</v>
@@ -2773,39 +2773,39 @@
         <v>63</v>
       </c>
       <c r="Q24" s="4">
-        <v>7.4733096085409206E-2</v>
+        <v>6.7669172932330796E-2</v>
       </c>
       <c r="R24" s="5">
-        <v>1807173</v>
+        <v>1852275</v>
       </c>
       <c r="S24" s="4">
-        <v>0.23620610623865501</v>
+        <v>0.215773848527579</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="8">
-        <v>1552</v>
+        <v>1536</v>
       </c>
       <c r="C25" s="5">
-        <v>21831062</v>
+        <v>22272296</v>
       </c>
       <c r="D25" s="8">
-        <v>843</v>
+        <v>931</v>
       </c>
       <c r="E25" s="5">
-        <v>7658716</v>
+        <v>8592429</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G25" s="7">
         <v>259</v>
@@ -2817,16 +2817,16 @@
         <v>14</v>
       </c>
       <c r="J25" s="4">
-        <v>9.0206185567010301E-3</v>
+        <v>9.1145833333333304E-3</v>
       </c>
       <c r="K25" s="5">
-        <v>564825</v>
+        <v>577523</v>
       </c>
       <c r="L25" s="4">
-        <v>2.58725388622871E-2</v>
+        <v>2.5930106173157899E-2</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N25" s="7">
         <v>216</v>
@@ -2838,104 +2838,104 @@
         <v>8</v>
       </c>
       <c r="Q25" s="4">
-        <v>9.4899169632265707E-3</v>
+        <v>8.5929108485499409E-3</v>
       </c>
       <c r="R25" s="5">
-        <v>478428</v>
+        <v>488322</v>
       </c>
       <c r="S25" s="4">
-        <v>6.2468434656670901E-2</v>
+        <v>5.6831659592415602E-2</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1529</v>
+      </c>
+      <c r="C26" s="5">
+        <v>21234889</v>
+      </c>
+      <c r="D26" s="8">
+        <v>994</v>
+      </c>
+      <c r="E26" s="5">
+        <v>9379456</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="7">
+        <v>46258</v>
+      </c>
+      <c r="H26" s="7">
+        <v>65206</v>
+      </c>
+      <c r="I26" s="8">
+        <v>947</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.61935905820797899</v>
+      </c>
+      <c r="K26" s="5">
+        <v>15005937</v>
+      </c>
+      <c r="L26" s="4">
+        <v>0.70666425428454005</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N26" s="7">
+        <v>34072</v>
+      </c>
+      <c r="O26" s="7">
+        <v>17604</v>
+      </c>
+      <c r="P26" s="8">
+        <v>663</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>0.66700201207243404</v>
+      </c>
+      <c r="R26" s="5">
+        <v>7389741</v>
+      </c>
+      <c r="S26" s="4">
+        <v>0.78786456272090799</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U26" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" s="8">
-        <v>1542</v>
-      </c>
-      <c r="C26" s="5">
-        <v>20802472</v>
-      </c>
-      <c r="D26" s="8">
-        <v>904</v>
-      </c>
-      <c r="E26" s="5">
-        <v>8316738</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G26" s="7">
-        <v>46243</v>
-      </c>
-      <c r="H26" s="7">
-        <v>65382</v>
-      </c>
-      <c r="I26" s="8">
-        <v>961</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0.62321660181582295</v>
-      </c>
-      <c r="K26" s="5">
-        <v>14650500</v>
-      </c>
-      <c r="L26" s="4">
-        <v>0.70426726208308299</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" s="7">
-        <v>33372</v>
-      </c>
-      <c r="O26" s="7">
-        <v>17361</v>
-      </c>
-      <c r="P26" s="8">
-        <v>630</v>
-      </c>
-      <c r="Q26" s="4">
-        <v>0.696902654867256</v>
-      </c>
-      <c r="R26" s="5">
-        <v>6621153</v>
-      </c>
-      <c r="S26" s="4">
-        <v>0.79612379276586498</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U26" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="8">
-        <v>1542</v>
+        <v>1529</v>
       </c>
       <c r="C27" s="5">
-        <v>20734474</v>
+        <v>21165826</v>
       </c>
       <c r="D27" s="8">
-        <v>904</v>
+        <v>994</v>
       </c>
       <c r="E27" s="5">
-        <v>8316788</v>
+        <v>9379506</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27" s="7">
         <v>16</v>
@@ -2947,16 +2947,16 @@
         <v>6</v>
       </c>
       <c r="J27" s="4">
-        <v>3.8910505836575798E-3</v>
+        <v>3.9241334205362896E-3</v>
       </c>
       <c r="K27" s="5">
-        <v>116360</v>
+        <v>119172</v>
       </c>
       <c r="L27" s="4">
-        <v>5.61190990424931E-3</v>
+        <v>5.63039684820238E-3</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N27" s="7">
         <v>5</v>
@@ -2968,39 +2968,39 @@
         <v>3</v>
       </c>
       <c r="Q27" s="4">
-        <v>3.3185840707964601E-3</v>
+        <v>3.01810865191146E-3</v>
       </c>
       <c r="R27" s="5">
-        <v>53335</v>
+        <v>54454</v>
       </c>
       <c r="S27" s="4">
-        <v>6.4129324926882796E-3</v>
+        <v>5.8056362456615504E-3</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="8">
-        <v>1544</v>
+        <v>1531</v>
       </c>
       <c r="C28" s="5">
-        <v>20775776</v>
+        <v>21208153</v>
       </c>
       <c r="D28" s="8">
-        <v>906</v>
+        <v>996</v>
       </c>
       <c r="E28" s="5">
-        <v>8350261</v>
+        <v>9414341</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G28" s="7">
         <v>1511</v>
@@ -3012,146 +3012,146 @@
         <v>126</v>
       </c>
       <c r="J28" s="4">
-        <v>8.1606217616580295E-2</v>
+        <v>8.2299150881776598E-2</v>
       </c>
       <c r="K28" s="5">
-        <v>2008397</v>
+        <v>2054462</v>
       </c>
       <c r="L28" s="4">
-        <v>9.6670131599416495E-2</v>
+        <v>9.68713305680131E-2</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N28" s="7">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="O28" s="7">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="P28" s="8">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Q28" s="4">
-        <v>0.123620309050772</v>
+        <v>0.11345381526104401</v>
       </c>
       <c r="R28" s="5">
-        <v>1808633</v>
+        <v>1899717</v>
       </c>
       <c r="S28" s="4">
-        <v>0.21659598424528201</v>
+        <v>0.20178969510452099</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1646</v>
+      </c>
+      <c r="C29" s="5">
+        <v>22632604</v>
+      </c>
+      <c r="D29" s="8">
+        <v>1076</v>
+      </c>
+      <c r="E29" s="5">
+        <v>9878412</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" s="7">
+        <v>53015</v>
+      </c>
+      <c r="H29" s="7">
+        <v>21150</v>
+      </c>
+      <c r="I29" s="8">
+        <v>789</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0.47934386391251499</v>
+      </c>
+      <c r="K29" s="5">
+        <v>14859125</v>
+      </c>
+      <c r="L29" s="4">
+        <v>0.65653625186036901</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N29" s="7">
+        <v>24613</v>
+      </c>
+      <c r="O29" s="7">
+        <v>13354</v>
+      </c>
+      <c r="P29" s="8">
+        <v>562</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>0.52230483271375405</v>
+      </c>
+      <c r="R29" s="5">
+        <v>6535261</v>
+      </c>
+      <c r="S29" s="4">
+        <v>0.66156999728296395</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U29" t="s">
         <v>63</v>
-      </c>
-      <c r="B29" s="8">
-        <v>1677</v>
-      </c>
-      <c r="C29" s="5">
-        <v>22336780</v>
-      </c>
-      <c r="D29" s="8">
-        <v>985</v>
-      </c>
-      <c r="E29" s="5">
-        <v>8787158</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G29" s="7">
-        <v>55717</v>
-      </c>
-      <c r="H29" s="7">
-        <v>20566</v>
-      </c>
-      <c r="I29" s="8">
-        <v>807</v>
-      </c>
-      <c r="J29" s="4">
-        <v>0.481216457960644</v>
-      </c>
-      <c r="K29" s="5">
-        <v>14667105</v>
-      </c>
-      <c r="L29" s="4">
-        <v>0.65663470741978003</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N29" s="7">
-        <v>24525</v>
-      </c>
-      <c r="O29" s="7">
-        <v>13331</v>
-      </c>
-      <c r="P29" s="8">
-        <v>560</v>
-      </c>
-      <c r="Q29" s="4">
-        <v>0.56852791878172504</v>
-      </c>
-      <c r="R29" s="5">
-        <v>6287773</v>
-      </c>
-      <c r="S29" s="4">
-        <v>0.71556389449239399</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U29" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="8">
-        <v>1705</v>
+        <v>1674</v>
       </c>
       <c r="C30" s="5">
-        <v>23062326</v>
+        <v>23375745</v>
       </c>
       <c r="D30" s="8">
-        <v>987</v>
+        <v>1078</v>
       </c>
       <c r="E30" s="5">
-        <v>8805280</v>
+        <v>9897003</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G30" s="7">
-        <v>22799</v>
+        <v>22901</v>
       </c>
       <c r="H30" s="7">
-        <v>2006</v>
+        <v>2186</v>
       </c>
       <c r="I30" s="8">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J30" s="4">
-        <v>7.0381231671554204E-2</v>
+        <v>7.1087216248506502E-2</v>
       </c>
       <c r="K30" s="5">
-        <v>5148370</v>
+        <v>5231676</v>
       </c>
       <c r="L30" s="4">
-        <v>0.22323723981700699</v>
+        <v>0.22380788291453299</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N30" s="7">
         <v>913</v>
@@ -3163,488 +3163,488 @@
         <v>55</v>
       </c>
       <c r="Q30" s="4">
-        <v>5.5724417426544999E-2</v>
+        <v>5.10204081632653E-2</v>
       </c>
       <c r="R30" s="5">
-        <v>1705869</v>
+        <v>1747527</v>
       </c>
       <c r="S30" s="4">
-        <v>0.19373251049370299</v>
+        <v>0.17657133174557901</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="8">
+        <v>1736</v>
+      </c>
+      <c r="C31" s="5">
+        <v>22617702</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1169</v>
+      </c>
+      <c r="E31" s="5">
+        <v>10458574</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="7">
+        <v>70377</v>
+      </c>
+      <c r="H31" s="7">
+        <v>97314</v>
+      </c>
+      <c r="I31" s="8">
+        <v>955</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0.55011520737327102</v>
+      </c>
+      <c r="K31" s="5">
+        <v>15762081</v>
+      </c>
+      <c r="L31" s="4">
+        <v>0.69689135527561497</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N31" s="7">
+        <v>26589</v>
+      </c>
+      <c r="O31" s="7">
+        <v>13625</v>
+      </c>
+      <c r="P31" s="8">
+        <v>634</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>0.54234388366124897</v>
+      </c>
+      <c r="R31" s="5">
+        <v>7882916</v>
+      </c>
+      <c r="S31" s="4">
+        <v>0.75372761143153899</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U31" t="s">
         <v>67</v>
-      </c>
-      <c r="B31" s="8">
-        <v>1760</v>
-      </c>
-      <c r="C31" s="5">
-        <v>22216921</v>
-      </c>
-      <c r="D31" s="8">
-        <v>1078</v>
-      </c>
-      <c r="E31" s="5">
-        <v>9355805</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="7">
-        <v>69160</v>
-      </c>
-      <c r="H31" s="7">
-        <v>98855</v>
-      </c>
-      <c r="I31" s="8">
-        <v>966</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0.548863636363636</v>
-      </c>
-      <c r="K31" s="5">
-        <v>15446736</v>
-      </c>
-      <c r="L31" s="4">
-        <v>0.69526897989149805</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N31" s="7">
-        <v>26436</v>
-      </c>
-      <c r="O31" s="7">
-        <v>13471</v>
-      </c>
-      <c r="P31" s="8">
-        <v>629</v>
-      </c>
-      <c r="Q31" s="4">
-        <v>0.58348794063079701</v>
-      </c>
-      <c r="R31" s="5">
-        <v>7396524</v>
-      </c>
-      <c r="S31" s="4">
-        <v>0.79058124875411495</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U31" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="8">
-        <v>1762</v>
+        <v>1738</v>
       </c>
       <c r="C32" s="5">
-        <v>22318550</v>
+        <v>22720448</v>
       </c>
       <c r="D32" s="8">
-        <v>1078</v>
+        <v>1171</v>
       </c>
       <c r="E32" s="5">
-        <v>9368938</v>
+        <v>10474050</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G32" s="7">
-        <v>5583</v>
+        <v>5623</v>
       </c>
       <c r="H32" s="7">
-        <v>4294</v>
+        <v>4337</v>
       </c>
       <c r="I32" s="8">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J32" s="4">
-        <v>6.46992054483541E-2</v>
+        <v>6.3291139240506306E-2</v>
       </c>
       <c r="K32" s="5">
-        <v>5964607</v>
+        <v>6093754</v>
       </c>
       <c r="L32" s="4">
-        <v>0.26724885801272902</v>
+        <v>0.26820571495773299</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N32" s="7">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="O32" s="7">
         <v>126</v>
       </c>
       <c r="P32" s="8">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q32" s="4">
-        <v>5.1948051948051903E-2</v>
+        <v>4.9530315969256999E-2</v>
       </c>
       <c r="R32" s="5">
-        <v>1523825</v>
+        <v>1562129</v>
       </c>
       <c r="S32" s="4">
-        <v>0.16264650273061801</v>
+        <v>0.14914278621927499</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1862</v>
+      </c>
+      <c r="C33" s="5">
+        <v>24302119</v>
+      </c>
+      <c r="D33" s="8">
+        <v>1255</v>
+      </c>
+      <c r="E33" s="5">
+        <v>10936563</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="7">
+        <v>68029</v>
+      </c>
+      <c r="H33" s="7">
+        <v>32195</v>
+      </c>
+      <c r="I33" s="8">
+        <v>1173</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0.62996777658431702</v>
+      </c>
+      <c r="K33" s="5">
+        <v>17969935</v>
+      </c>
+      <c r="L33" s="4">
+        <v>0.73943901764286402</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N33" s="7">
+        <v>31135</v>
+      </c>
+      <c r="O33" s="7">
+        <v>17370</v>
+      </c>
+      <c r="P33" s="8">
+        <v>867</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>0.69083665338645395</v>
+      </c>
+      <c r="R33" s="5">
+        <v>8938409</v>
+      </c>
+      <c r="S33" s="4">
+        <v>0.81729598229352296</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U33" t="s">
         <v>71</v>
-      </c>
-      <c r="B33" s="8">
-        <v>1931</v>
-      </c>
-      <c r="C33" s="5">
-        <v>23990311</v>
-      </c>
-      <c r="D33" s="8">
-        <v>1222</v>
-      </c>
-      <c r="E33" s="5">
-        <v>9996261</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="7">
-        <v>70715</v>
-      </c>
-      <c r="H33" s="7">
-        <v>31185</v>
-      </c>
-      <c r="I33" s="8">
-        <v>1219</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0.631279129984464</v>
-      </c>
-      <c r="K33" s="5">
-        <v>17681031</v>
-      </c>
-      <c r="L33" s="4">
-        <v>0.737007160932594</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N33" s="7">
-        <v>35534</v>
-      </c>
-      <c r="O33" s="7">
-        <v>17480</v>
-      </c>
-      <c r="P33" s="8">
-        <v>922</v>
-      </c>
-      <c r="Q33" s="4">
-        <v>0.75450081833060501</v>
-      </c>
-      <c r="R33" s="5">
-        <v>8470069</v>
-      </c>
-      <c r="S33" s="4">
-        <v>0.84732371433678999</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U33" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="8">
-        <v>1931</v>
+        <v>1862</v>
       </c>
       <c r="C34" s="5">
-        <v>24032469</v>
+        <v>24345914</v>
       </c>
       <c r="D34" s="8">
-        <v>1222</v>
+        <v>1255</v>
       </c>
       <c r="E34" s="5">
-        <v>9998478</v>
+        <v>10939501</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G34" s="7">
-        <v>2395</v>
+        <v>2393</v>
       </c>
       <c r="H34" s="7">
-        <v>1469</v>
+        <v>1457</v>
       </c>
       <c r="I34" s="8">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J34" s="4">
-        <v>4.0911444847229403E-2</v>
+        <v>4.13533834586466E-2</v>
       </c>
       <c r="K34" s="5">
-        <v>4898783</v>
+        <v>5016632</v>
       </c>
       <c r="L34" s="4">
-        <v>0.20384018803894</v>
+        <v>0.20605642490973999</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N34" s="7">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O34" s="7">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="P34" s="8">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q34" s="4">
-        <v>3.1914893617021198E-2</v>
+        <v>2.9482071713147401E-2</v>
       </c>
       <c r="R34" s="5">
-        <v>1256437</v>
+        <v>1283301</v>
       </c>
       <c r="S34" s="4">
-        <v>0.12566282588209901</v>
+        <v>0.117308915644324</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2049</v>
+      </c>
+      <c r="C35" s="5">
+        <v>27257560</v>
+      </c>
+      <c r="D35" s="8">
+        <v>1415</v>
+      </c>
+      <c r="E35" s="5">
+        <v>12682870</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35" s="7">
+        <v>99137</v>
+      </c>
+      <c r="H35" s="7">
+        <v>34803</v>
+      </c>
+      <c r="I35" s="8">
+        <v>1160</v>
+      </c>
+      <c r="J35" s="4">
+        <v>0.566129819424109</v>
+      </c>
+      <c r="K35" s="5">
+        <v>19979368</v>
+      </c>
+      <c r="L35" s="4">
+        <v>0.73298446375977899</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N35" s="7">
+        <v>57926</v>
+      </c>
+      <c r="O35" s="7">
+        <v>18650</v>
+      </c>
+      <c r="P35" s="8">
+        <v>859</v>
+      </c>
+      <c r="Q35" s="4">
+        <v>0.60706713780918697</v>
+      </c>
+      <c r="R35" s="5">
+        <v>9865668</v>
+      </c>
+      <c r="S35" s="4">
+        <v>0.77787346239455202</v>
+      </c>
+      <c r="T35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U35" t="s">
         <v>74</v>
-      </c>
-      <c r="B35" s="8">
-        <v>2055</v>
-      </c>
-      <c r="C35" s="5">
-        <v>26682903</v>
-      </c>
-      <c r="D35" s="8">
-        <v>1324</v>
-      </c>
-      <c r="E35" s="5">
-        <v>11553928</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" s="7">
-        <v>93883</v>
-      </c>
-      <c r="H35" s="7">
-        <v>34260</v>
-      </c>
-      <c r="I35" s="8">
-        <v>1147</v>
-      </c>
-      <c r="J35" s="4">
-        <v>0.55815085158150801</v>
-      </c>
-      <c r="K35" s="5">
-        <v>19473261</v>
-      </c>
-      <c r="L35" s="4">
-        <v>0.72980293785874795</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N35" s="7">
-        <v>53457</v>
-      </c>
-      <c r="O35" s="7">
-        <v>18912</v>
-      </c>
-      <c r="P35" s="8">
-        <v>842</v>
-      </c>
-      <c r="Q35" s="4">
-        <v>0.63595166163141903</v>
-      </c>
-      <c r="R35" s="5">
-        <v>9388512</v>
-      </c>
-      <c r="S35" s="4">
-        <v>0.81258183364133796</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U35" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="8">
-        <v>2059</v>
+        <v>2053</v>
       </c>
       <c r="C36" s="5">
-        <v>27313181</v>
+        <v>27901769</v>
       </c>
       <c r="D36" s="8">
-        <v>1327</v>
+        <v>1418</v>
       </c>
       <c r="E36" s="5">
-        <v>11606475</v>
+        <v>12739484</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G36" s="7">
-        <v>22400</v>
+        <v>22897</v>
       </c>
       <c r="H36" s="7">
-        <v>8470</v>
+        <v>8967</v>
       </c>
       <c r="I36" s="8">
         <v>127</v>
       </c>
       <c r="J36" s="4">
-        <v>6.1680427391937798E-2</v>
+        <v>6.18606916707257E-2</v>
       </c>
       <c r="K36" s="5">
-        <v>8674266</v>
+        <v>8883301</v>
       </c>
       <c r="L36" s="4">
-        <v>0.31758534459973697</v>
+        <v>0.31837769856097597</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N36" s="7">
-        <v>1845</v>
+        <v>2257</v>
       </c>
       <c r="O36" s="7">
-        <v>634</v>
+        <v>939</v>
       </c>
       <c r="P36" s="8">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q36" s="4">
-        <v>3.9939713639788897E-2</v>
+        <v>3.8787023977432999E-2</v>
       </c>
       <c r="R36" s="5">
-        <v>1630172</v>
+        <v>1691152</v>
       </c>
       <c r="S36" s="4">
-        <v>0.14045366918034899</v>
+        <v>0.13274886172783701</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2191</v>
+      </c>
+      <c r="C37" s="5">
+        <v>28896970</v>
+      </c>
+      <c r="D37" s="8">
+        <v>1523</v>
+      </c>
+      <c r="E37" s="5">
+        <v>13697551</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="7">
+        <v>131895</v>
+      </c>
+      <c r="H37" s="7">
+        <v>131091</v>
+      </c>
+      <c r="I37" s="8">
+        <v>1370</v>
+      </c>
+      <c r="J37" s="4">
+        <v>0.62528525787311695</v>
+      </c>
+      <c r="K37" s="5">
+        <v>21838777</v>
+      </c>
+      <c r="L37" s="4">
+        <v>0.75574625990198896</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N37" s="7">
+        <v>47017</v>
+      </c>
+      <c r="O37" s="7">
+        <v>23242</v>
+      </c>
+      <c r="P37" s="8">
+        <v>1007</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>0.66119500984898205</v>
+      </c>
+      <c r="R37" s="5">
+        <v>10978216</v>
+      </c>
+      <c r="S37" s="4">
+        <v>0.80147290563108597</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U37" t="s">
         <v>78</v>
-      </c>
-      <c r="B37" s="8">
-        <v>2205</v>
-      </c>
-      <c r="C37" s="5">
-        <v>28362003</v>
-      </c>
-      <c r="D37" s="8">
-        <v>1432</v>
-      </c>
-      <c r="E37" s="5">
-        <v>12546038</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G37" s="7">
-        <v>131696</v>
-      </c>
-      <c r="H37" s="7">
-        <v>129836</v>
-      </c>
-      <c r="I37" s="8">
-        <v>1381</v>
-      </c>
-      <c r="J37" s="4">
-        <v>0.62630385487528295</v>
-      </c>
-      <c r="K37" s="5">
-        <v>21394510</v>
-      </c>
-      <c r="L37" s="4">
-        <v>0.75433706145507395</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N37" s="7">
-        <v>46319</v>
-      </c>
-      <c r="O37" s="7">
-        <v>22534</v>
-      </c>
-      <c r="P37" s="8">
-        <v>983</v>
-      </c>
-      <c r="Q37" s="4">
-        <v>0.68645251396647999</v>
-      </c>
-      <c r="R37" s="5">
-        <v>10467719</v>
-      </c>
-      <c r="S37" s="4">
-        <v>0.83434459548105899</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U37" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="G39" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
@@ -3652,7 +3652,7 @@
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
       <c r="N39" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="O39" s="11"/>
       <c r="P39" s="11"/>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -3704,7 +3704,7 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>

</xml_diff>

<commit_message>
Include new Bitcoin versions
</commit_message>
<xml_diff>
--- a/logDirectoryOutput.xlsx
+++ b/logDirectoryOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Simeon\Documents\GitHub\bitcoin-version-compare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simeo\Documents\GitHub\bitcoin-version-compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2708DA-6478-40EA-9523-F9B4555191B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23193BC-2141-4683-95BA-5E40C88D243C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="135" windowWidth="18090" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="1890" windowWidth="21900" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logDirectoryOutput" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="130">
   <si>
     <t>Num all files</t>
   </si>
@@ -298,6 +298,120 @@
   <si>
     <t>Comparison across code files
 (cpp, py, c, h, sh, sol, go, c, js, java)</t>
+  </si>
+  <si>
+    <t>bitcoin-22.1</t>
+  </si>
+  <si>
+    <t>.cpp (516), .h (450), .py (234), .md (181), .ts (97), .png (93), .json (92), .cc (89), .sh (73),  (65), .mk (38), .patch (28), .hex (28), .in (23), .svg (21), .c (19), .ui (19), .vcxproj (17), .m4 (16), .yml (13), .include (13), .txt (8), .1 (6), .rc (6), .sage (6), .am (5), .xpm (5), .ac (3), .bash-completion (3), .bash (3), .conf (3), .ico (3), .mm (3), .targets (2), .pro (2), .bmp (2), .raw (2), .capnp (2), .html (2), .qrc (2), .yapf (1), .sln (1), .supp (1), .scm (1), .init (1), .openrc (1), .openrcconf (1), .service (1), .plist (1), .cfg (1), .cert (1), .guess (1), .sub (1), .cmake (1), .xml (1), .gradle (1), .properties (1), .java (1), .xlf (1), .ttf (1), .icns (1), .dockerfile (1), .s (1), .csv (1)</t>
+  </si>
+  <si>
+    <t>.cpp (516), .h (450), .py (234), .sh (73), .c (19), .java (1)</t>
+  </si>
+  <si>
+    <t>bitcoin-23.0</t>
+  </si>
+  <si>
+    <t>.cpp (559), .h (482), .py (257), .md (195), .png (98), .json (94), .ts (94), .cc (89), .sh (74),  (63), .mk (51), .patch (30), .hex (29), .in (24), .svg (20), .ui (19), .m4 (18), .vcxproj (17), .c (17), .include (15), .txt (9), .sage (9), .yml (7), .am (6), .1 (6), .rc (6), .xpm (5), .ac (4), .bash-completion (3), .bash (3), .conf (3), .bt (3), .ico (3), .mm (3), .targets (2), .pro (2), .bmp (2), .raw (2), .capnp (2), .html (2), .dockerfile (2), .qrc (2), .xml (2), .yapf (1), .sln (1), .supp (1), .scm (1), .init (1), .openrc (1), .openrcconf (1), .service (1), .cfg (1), .tiff (1), .cert (1), .guess (1), .sub (1), .cmake (1), .gradle (1), .properties (1), .java (1), .xlf (1), .ttf (1), .icns (1), .s (1), .csv (1)</t>
+  </si>
+  <si>
+    <t>.cpp (559), .h (482), .py (257), .sh (74), .c (17), .java (1)</t>
+  </si>
+  <si>
+    <t>bitcoin-23.1</t>
+  </si>
+  <si>
+    <t>.cpp (561), .h (482), .py (258), .md (196), .ts (99), .png (98), .json (94), .cc (89), .sh (74),  (67), .mk (51), .patch (29), .hex (29), .in (24), .svg (20), .m4 (19), .ui (19), .vcxproj (17), .c (17), .include (15), .txt (9), .sage (9), .yml (8), .am (6), .1 (6), .rc (6), .xpm (5), .ac (4), .bash-completion (3), .bash (3), .conf (3), .bt (3), .ico (3), .mm (3), .targets (2), .pro (2), .bmp (2), .raw (2), .capnp (2), .html (2), .dockerfile (2), .qrc (2), .xml (2), .yapf (1), .sln (1), .supp (1), .scm (1), .init (1), .openrc (1), .openrcconf (1), .service (1), .plist (1), .cfg (1), .tiff (1), .cert (1), .guess (1), .sub (1), .cmake (1), .gradle (1), .properties (1), .java (1), .xlf (1), .ttf (1), .icns (1), .s (1), .csv (1)</t>
+  </si>
+  <si>
+    <t>.cpp (561), .h (482), .py (258), .sh (74), .c (17), .java (1)</t>
+  </si>
+  <si>
+    <t>bitcoin-24.0.1</t>
+  </si>
+  <si>
+    <t>.cpp (599), .h (507), .py (297), .md (198), .png (98), .ts (98), .json (94), .cc (89),  (66), .sh (50), .mk (50), .patch (35), .hex (29), .in (23), .c (22), .svg (20), .ui (19), .m4 (18), .vcxproj (16), .include (15), .sage (9), .txt (8), .yml (7), .1 (6), .rc (6), .am (5), .xpm (5), .ac (3), .bash-completion (3), .bash (3), .conf (3), .bt (3), .ico (3), .mm (3), .targets (2), .pro (2), .bmp (2), .raw (2), .capnp (2), .html (2), .dockerfile (2), .qrc (2), .xml (2), .yapf (1), .sln (1), .bat (1), .supp (1), .imp (1), .scm (1), .init (1), .openrc (1), .openrcconf (1), .service (1), .plist (1), .cfg (1), .tiff (1), .cert (1), .guess (1), .sub (1), .cmake (1), .gradle (1), .properties (1), .java (1), .xlf (1), .ttf (1), .icns (1), .s (1), .csv (1)</t>
+  </si>
+  <si>
+    <t>.cpp (599), .h (507), .py (297), .sh (50), .c (22), .java (1)</t>
+  </si>
+  <si>
+    <t>Code file extenension histogram</t>
+  </si>
+  <si>
+    <t>.h (233), .cpp (179), .py (41), .sh (16), .c (7), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (233), .cpp (180), .py (43), .sh (16), .c (7), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (233), .cpp (180), .py (45), .sh (16), .c (7), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (249), .cpp (189), .py (61), .sh (16), .c (8), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (249), .cpp (189), .py (63), .sh (16), .c (8), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (267), .cpp (203), .py (85), .sh (15), .c (13), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (268), .cpp (205), .py (89), .sh (15), .c (13), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (276), .cpp (214), .py (101), .c (16), .sh (14), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (276), .cpp (214), .py (106), .c (16), .sh (14), .java (1)</t>
+  </si>
+  <si>
+    <t>.h (274), .cpp (213), .py (106), .c (18), .sh (14), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (287), .cpp (232), .py (112), .c (18), .sh (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (287), .cpp (233), .py (112), .c (18), .sh (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (297), .cpp (243), .py (120), .sh (19), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (296), .cpp (243), .py (123), .sh (19), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (302), .cpp (256), .py (133), .sh (23), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (302), .cpp (257), .py (134), .sh (23), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (317), .cpp (281), .py (148), .sh (32), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (317), .cpp (281), .py (150), .sh (32), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (339), .cpp (309), .py (165), .sh (45), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (339), .cpp (310), .py (166), .sh (45), .c (17), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (365), .cpp (345), .py (174), .sh (64), .c (18), .java (4)</t>
+  </si>
+  <si>
+    <t>.h (390), .cpp (355), .py (190), .sh (70), .c (19), .java (4)</t>
+  </si>
+  <si>
+    <t>.cpp (466), .h (417), .py (209), .sh (75), .c (19)</t>
+  </si>
+  <si>
+    <t>.cpp (467), .h (418), .py (210), .sh (75), .c (19)</t>
+  </si>
+  <si>
+    <t>.cpp (515), .h (450), .py (233), .sh (73), .c (19), .java (1)</t>
   </si>
 </sst>
 </file>
@@ -1205,9 +1319,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U43"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:V1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1225,9 +1341,10 @@
     <col min="19" max="19" width="13.7109375" style="3" customWidth="1"/>
     <col min="20" max="20" width="1.7109375" style="1" customWidth="1"/>
     <col min="21" max="21" width="255.5703125" customWidth="1"/>
+    <col min="22" max="22" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
@@ -1291,8 +1408,11 @@
       <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1356,8 +1476,11 @@
       <c r="U2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1421,8 +1544,11 @@
       <c r="U3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1486,8 +1612,11 @@
       <c r="U4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -1551,8 +1680,11 @@
       <c r="U5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1616,8 +1748,11 @@
       <c r="U6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1681,8 +1816,11 @@
       <c r="U7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -1746,8 +1884,11 @@
       <c r="U8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1811,8 +1952,11 @@
       <c r="U9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1876,8 +2020,11 @@
       <c r="U10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -1941,8 +2088,11 @@
       <c r="U11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -2006,8 +2156,11 @@
       <c r="U12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -2071,8 +2224,11 @@
       <c r="U13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -2136,8 +2292,11 @@
       <c r="U14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -2201,8 +2360,11 @@
       <c r="U15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -2266,8 +2428,11 @@
       <c r="U16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -2331,8 +2496,11 @@
       <c r="U17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
@@ -2396,8 +2564,11 @@
       <c r="U18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -2461,8 +2632,11 @@
       <c r="U19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -2526,8 +2700,11 @@
       <c r="U20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -2591,8 +2768,11 @@
       <c r="U21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2656,8 +2836,11 @@
       <c r="U22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -2721,8 +2904,11 @@
       <c r="U23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -2786,8 +2972,11 @@
       <c r="U24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
@@ -2851,8 +3040,11 @@
       <c r="U25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -2916,8 +3108,11 @@
       <c r="U26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
@@ -2981,8 +3176,11 @@
       <c r="U27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -3046,8 +3244,11 @@
       <c r="U28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -3111,8 +3312,11 @@
       <c r="U29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
@@ -3176,8 +3380,11 @@
       <c r="U30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
@@ -3241,8 +3448,11 @@
       <c r="U31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
@@ -3306,8 +3516,11 @@
       <c r="U32" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
@@ -3371,8 +3584,11 @@
       <c r="U33" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -3436,8 +3652,11 @@
       <c r="U34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -3501,8 +3720,11 @@
       <c r="U35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -3566,8 +3788,11 @@
       <c r="U36" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
@@ -3631,123 +3856,398 @@
       <c r="U37" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="8">
+        <v>2217</v>
+      </c>
+      <c r="C38" s="5">
+        <v>29216471</v>
+      </c>
+      <c r="D38" s="8">
+        <v>1526</v>
+      </c>
+      <c r="E38" s="5">
+        <v>13393499</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="7">
+        <v>29453</v>
+      </c>
+      <c r="H38" s="7">
+        <v>9957</v>
+      </c>
+      <c r="I38" s="8">
+        <v>137</v>
+      </c>
+      <c r="J38" s="4">
+        <v>6.1795218764095598E-2</v>
+      </c>
+      <c r="K38" s="5">
+        <v>9166031</v>
+      </c>
+      <c r="L38" s="4">
+        <v>0.31372820488826297</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N38" s="7">
+        <v>445</v>
+      </c>
+      <c r="O38" s="7">
+        <v>133</v>
+      </c>
+      <c r="P38" s="8">
+        <v>35</v>
+      </c>
+      <c r="Q38" s="4">
+        <v>2.29357798165137E-2</v>
+      </c>
+      <c r="R38" s="5">
+        <v>989575</v>
+      </c>
+      <c r="S38" s="4">
+        <v>7.3884725716558394E-2</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U38" t="s">
+        <v>93</v>
+      </c>
+      <c r="V38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="8">
+        <v>2355</v>
+      </c>
+      <c r="C39" s="5">
+        <v>35666095</v>
+      </c>
+      <c r="D39" s="8">
+        <v>1629</v>
+      </c>
+      <c r="E39" s="5">
+        <v>18844898</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="7">
+        <v>166281</v>
+      </c>
+      <c r="H39" s="7">
+        <v>114755</v>
+      </c>
+      <c r="I39" s="8">
+        <v>1429</v>
+      </c>
+      <c r="J39" s="4">
+        <v>0.60679405520169805</v>
+      </c>
+      <c r="K39" s="5">
+        <v>28110854</v>
+      </c>
+      <c r="L39" s="4">
+        <v>0.78816741782356603</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N39" s="7">
+        <v>74606</v>
+      </c>
+      <c r="O39" s="7">
+        <v>19628</v>
+      </c>
+      <c r="P39" s="8">
+        <v>1048</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>0.64333947206875297</v>
+      </c>
+      <c r="R39" s="5">
+        <v>16178915</v>
+      </c>
+      <c r="S39" s="4">
+        <v>0.85853025046885301</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U39" t="s">
+        <v>96</v>
+      </c>
+      <c r="V39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2370</v>
+      </c>
+      <c r="C40" s="5">
+        <v>36250861</v>
+      </c>
+      <c r="D40" s="8">
+        <v>1633</v>
+      </c>
+      <c r="E40" s="5">
+        <v>18519498</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="7">
+        <v>26592</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1903</v>
+      </c>
+      <c r="I40" s="8">
+        <v>109</v>
+      </c>
+      <c r="J40" s="4">
+        <v>4.5991561181434597E-2</v>
+      </c>
+      <c r="K40" s="5">
+        <v>8673361</v>
+      </c>
+      <c r="L40" s="4">
+        <v>0.239259448210071</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N40" s="7">
+        <v>1077</v>
+      </c>
+      <c r="O40" s="7">
+        <v>110</v>
+      </c>
+      <c r="P40" s="8">
+        <v>18</v>
+      </c>
+      <c r="Q40" s="4">
+        <v>1.1022657685241801E-2</v>
+      </c>
+      <c r="R40" s="5">
+        <v>509963</v>
+      </c>
+      <c r="S40" s="4">
+        <v>2.7536545537033399E-2</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U40" t="s">
+        <v>99</v>
+      </c>
+      <c r="V40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="8">
+        <v>2453</v>
+      </c>
+      <c r="C41" s="5">
+        <v>37204360</v>
+      </c>
+      <c r="D41" s="8">
+        <v>1716</v>
+      </c>
+      <c r="E41" s="5">
+        <v>19517166</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G41" s="7">
+        <v>57126</v>
+      </c>
+      <c r="H41" s="7">
+        <v>37930</v>
+      </c>
+      <c r="I41" s="8">
+        <v>1128</v>
+      </c>
+      <c r="J41" s="4">
+        <v>0.45984508764777798</v>
+      </c>
+      <c r="K41" s="5">
+        <v>26704283</v>
+      </c>
+      <c r="L41" s="4">
+        <v>0.717772943816262</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N41" s="7">
+        <v>41158</v>
+      </c>
+      <c r="O41" s="7">
+        <v>16694</v>
+      </c>
+      <c r="P41" s="8">
+        <v>807</v>
+      </c>
+      <c r="Q41" s="4">
+        <v>0.47027972027971998</v>
+      </c>
+      <c r="R41" s="5">
+        <v>14516049</v>
+      </c>
+      <c r="S41" s="4">
+        <v>0.74375803331282797</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U41" t="s">
+        <v>102</v>
+      </c>
+      <c r="V41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="G39" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="N39" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
-      <c r="G43" s="11"/>
+      <c r="G43" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
-      <c r="N43" s="11"/>
+      <c r="N43" s="12" t="s">
+        <v>91</v>
+      </c>
       <c r="O43" s="11"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="11"/>
       <c r="R43" s="11"/>
       <c r="S43" s="11"/>
     </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G39:L43"/>
-    <mergeCell ref="N39:S43"/>
-    <mergeCell ref="B39:E43"/>
+    <mergeCell ref="G43:L47"/>
+    <mergeCell ref="N43:S47"/>
+    <mergeCell ref="B43:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3755,312 +4255,468 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F98823F-F407-46D8-AA59-6586EBBE7321}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="255.5703125" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B32" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B34" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B35" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B36" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>78</v>
+      </c>
+      <c r="C37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>